<commit_message>
update for solving erros in the project
</commit_message>
<xml_diff>
--- a/doc/Dictionary of Telco data.xlsx
+++ b/doc/Dictionary of Telco data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erico\OneDrive\Documentos\Projeto-Eric-Churn\Telco-Customer-Churn\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erico\Documents\projeto classificacao\Telco-Customer-Churn\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10911DA-1F9D-4BBC-9B4F-2DBB07CD1F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1DB85-2E10-49DB-A612-B8D1351A21AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -151,14 +151,14 @@
     <t>Clientes que saíram (yes) ou não (no)</t>
   </si>
   <si>
-    <t>Número de serviços em posse</t>
+    <t>Número de meses que passou na empresa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -178,6 +178,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="21">
     <fill>
@@ -313,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -335,6 +343,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,16 +565,16 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="1" max="1" width="64.88671875" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -605,7 +614,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -637,7 +646,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -669,7 +678,7 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -701,7 +710,7 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -733,7 +742,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -765,11 +774,11 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="8"/>
@@ -797,7 +806,7 @@
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -829,7 +838,7 @@
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
@@ -861,7 +870,7 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
@@ -893,7 +902,7 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -925,7 +934,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>23</v>
       </c>
@@ -957,7 +966,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>25</v>
       </c>
@@ -989,7 +998,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1030,7 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -1053,7 +1062,7 @@
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
@@ -1085,7 +1094,7 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>33</v>
       </c>
@@ -1117,7 +1126,7 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
@@ -1149,7 +1158,7 @@
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1181,7 +1190,7 @@
       <c r="Y20" s="18"/>
       <c r="Z20" s="18"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>39</v>
       </c>
@@ -1213,7 +1222,7 @@
       <c r="Y21" s="19"/>
       <c r="Z21" s="19"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
@@ -1247,5 +1256,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>